<commit_message>
Validation of the order with empty cart and filled form: fixed
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -42,6 +42,15 @@
     <t xml:space="preserve">Une page “produit” qui affiche (de manière dynamique) les détails du produit sur
 lequel l'utilisateur a cliqué depuis la page d’accueil. Depuis cette page, l’utilisateur
 peut sélectionner une quantité, une couleur, et ajouter le produit à son panier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliquer sur différents produits. Ouvrir les menus déroulants / Taper des données. Cliquer sur le bouton d'ajout au panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voire une liste de couleur, pouvoir renseigner une quantité d'article. Possibilité de l'ajouter au panier </t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
   <si>
     <t xml:space="preserve">Une page “panier”. Celle-ci contient plusieurs parties :
@@ -52,12 +61,24 @@
 back-end. Par exemple, pas de chiffre dans un champ prénom.</t>
   </si>
   <si>
+    <t xml:space="preserve">Modifier les quantités d'un produit, le supprimer. Rentrer les informations adéquates par le formulaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La quantité totald d'articles ainsi que le prix total doivent être automatiquement calculés et affichés, au gré des modifications et suppressions. Le formulaire doit avertir si les informations entrées sont inadéquats.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Une page “confirmation” :
 ○ Un message de confirmation de commande, remerciant l'utilisateur pour sa
 commande, et indiquant l'identifiant de commande envoyé par l’API.</t>
   </si>
   <si>
-    <t>...</t>
+    <t xml:space="preserve">Analyser la page pour vérifier si le numéro de commande est bien renseigné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoir le numéro de commande bien renseigné</t>
+  </si>
+  <si>
+    <t>Ok</t>
   </si>
 </sst>
 </file>
@@ -100,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -274,69 +295,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -372,18 +335,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -897,7 +848,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0" zoomScale="100">
+    <sheetView topLeftCell="A14" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -948,155 +899,67 @@
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" ht="198">
       <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" ht="82.5">
       <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
+        <v>15</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" ht="16.5">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" ht="16.5">
-      <c r="A7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" ht="16.5">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" ht="16.5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" ht="16.5">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" ht="16.5">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" ht="16.5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" ht="16.5">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" ht="16.5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" ht="16.5">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" ht="16.5">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" ht="16.5">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" ht="16.5">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" ht="16.5">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" ht="16.5">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" ht="16.5">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" ht="16.5">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
-    </row>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>